<commit_message>
Improved CreateTransaction and DetailTransaction areas
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Accounts: try to do more large active/hidden accounts toggler</t>
+  </si>
+  <si>
+    <t>Complete CreateTransaction() method</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
   <dimension ref="B1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +524,9 @@
       </c>
       <c r="C12" s="2">
         <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>